<commit_message>
[JDZ] FIN du TP
</commit_message>
<xml_diff>
--- a/Resultats.xlsx
+++ b/Resultats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>traces</t>
   </si>
@@ -32,6 +32,24 @@
   </si>
   <si>
     <t>nbr de Write</t>
+  </si>
+  <si>
+    <t>multTrace10x10Miss</t>
+  </si>
+  <si>
+    <t>multTrace10x10CopyInMemory</t>
+  </si>
+  <si>
+    <t>multTrace10x10Success</t>
+  </si>
+  <si>
+    <t>mergesort2000TraceMiss</t>
+  </si>
+  <si>
+    <t>mergesort2000TraceCopyInMemory</t>
+  </si>
+  <si>
+    <t>mergesort2000Trace10x10Success</t>
   </si>
 </sst>
 </file>
@@ -282,11 +300,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="564287064"/>
-        <c:axId val="564283144"/>
+        <c:axId val="324859504"/>
+        <c:axId val="324864600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="564287064"/>
+        <c:axId val="324859504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -390,7 +408,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="564283144"/>
+        <c:crossAx val="324864600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -398,7 +416,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="564283144"/>
+        <c:axId val="324864600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +523,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="564287064"/>
+        <c:crossAx val="324859504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -569,7 +587,14 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.36832740600989655"/>
+          <c:y val="0.15740740740740741"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -692,49 +717,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>969254</c:v>
+                  <c:v>894504</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>290914</c:v>
+                  <c:v>326599</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>990318</c:v>
+                  <c:v>903224</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>258048</c:v>
+                  <c:v>280168</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>242610</c:v>
+                  <c:v>187245</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>315315</c:v>
+                  <c:v>194940</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1268672</c:v>
+                  <c:v>1082576</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>344400</c:v>
+                  <c:v>184016</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>642957</c:v>
+                  <c:v>199869</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>782510</c:v>
+                  <c:v>231795</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>867726</c:v>
+                  <c:v>220410</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>649080</c:v>
+                  <c:v>204660</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>648394</c:v>
+                  <c:v>275329</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1167797</c:v>
+                  <c:v>901930</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1851040</c:v>
+                  <c:v>1551160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -750,11 +775,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="568211752"/>
-        <c:axId val="568211360"/>
+        <c:axId val="159878112"/>
+        <c:axId val="380646136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="568211752"/>
+        <c:axId val="159878112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -858,7 +883,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="568211360"/>
+        <c:crossAx val="380646136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -866,7 +891,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="568211360"/>
+        <c:axId val="380646136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -973,7 +998,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="568211752"/>
+        <c:crossAx val="159878112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1160,49 +1185,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>3263</c:v>
+                  <c:v>1976</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2951</c:v>
+                  <c:v>1326</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2632</c:v>
+                  <c:v>1064</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2926</c:v>
+                  <c:v>868</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2925</c:v>
+                  <c:v>765</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3210</c:v>
+                  <c:v>660</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2944</c:v>
+                  <c:v>608</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3216</c:v>
+                  <c:v>544</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5049</c:v>
+                  <c:v>527</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4624</c:v>
+                  <c:v>493</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5436</c:v>
+                  <c:v>468</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5508</c:v>
+                  <c:v>432</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4883</c:v>
+                  <c:v>418</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6954</c:v>
+                  <c:v>399</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4660</c:v>
+                  <c:v>380</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1218,11 +1243,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="568213712"/>
-        <c:axId val="568214496"/>
+        <c:axId val="380638688"/>
+        <c:axId val="380639864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="568213712"/>
+        <c:axId val="380638688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1329,7 +1354,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="568214496"/>
+        <c:crossAx val="380639864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1337,7 +1362,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="568214496"/>
+        <c:axId val="380639864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,7 +1474,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="568213712"/>
+        <c:crossAx val="380638688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3171,15 +3196,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:colOff>221974</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>43690</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>482462</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>119890</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3201,15 +3226,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:colOff>349526</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>31266</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>610014</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>107466</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3231,15 +3256,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:colOff>292376</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>167101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>552864</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>52801</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3550,13 +3575,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3615,49 +3640,49 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>3263</v>
+        <v>1976</v>
       </c>
       <c r="C2">
-        <v>2951</v>
+        <v>1326</v>
       </c>
       <c r="D2">
-        <v>2632</v>
+        <v>1064</v>
       </c>
       <c r="E2">
-        <v>2926</v>
+        <v>868</v>
       </c>
       <c r="F2">
-        <v>2925</v>
+        <v>765</v>
       </c>
       <c r="G2">
-        <v>3210</v>
+        <v>660</v>
       </c>
       <c r="H2">
-        <v>2944</v>
+        <v>608</v>
       </c>
       <c r="I2">
-        <v>3216</v>
+        <v>544</v>
       </c>
       <c r="J2">
-        <v>5049</v>
+        <v>527</v>
       </c>
       <c r="K2">
-        <v>4624</v>
+        <v>493</v>
       </c>
       <c r="L2">
-        <v>5436</v>
+        <v>468</v>
       </c>
       <c r="M2">
-        <v>5508</v>
+        <v>432</v>
       </c>
       <c r="N2">
-        <v>4883</v>
+        <v>418</v>
       </c>
       <c r="O2">
-        <v>6954</v>
+        <v>399</v>
       </c>
       <c r="P2">
-        <v>4660</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -3665,49 +3690,49 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>969254</v>
+        <v>894504</v>
       </c>
       <c r="C3">
-        <v>290914</v>
+        <v>326599</v>
       </c>
       <c r="D3">
-        <v>990318</v>
+        <v>903224</v>
       </c>
       <c r="E3">
-        <v>258048</v>
+        <v>280168</v>
       </c>
       <c r="F3">
-        <v>242610</v>
+        <v>187245</v>
       </c>
       <c r="G3">
-        <v>315315</v>
+        <v>194940</v>
       </c>
       <c r="H3">
-        <v>1268672</v>
+        <v>1082576</v>
       </c>
       <c r="I3">
-        <v>344400</v>
+        <v>184016</v>
       </c>
       <c r="J3">
-        <v>642957</v>
+        <v>199869</v>
       </c>
       <c r="K3">
-        <v>782510</v>
+        <v>231795</v>
       </c>
       <c r="L3">
-        <v>867726</v>
+        <v>220410</v>
       </c>
       <c r="M3">
-        <v>649080</v>
+        <v>204660</v>
       </c>
       <c r="N3">
-        <v>648394</v>
+        <v>275329</v>
       </c>
       <c r="O3">
-        <v>1167797</v>
+        <v>901930</v>
       </c>
       <c r="P3">
-        <v>1851040</v>
+        <v>1551160</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -3760,19 +3785,319 @@
         <v>34607980</v>
       </c>
     </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>152</v>
+      </c>
+      <c r="C5">
+        <v>102</v>
+      </c>
+      <c r="D5">
+        <v>76</v>
+      </c>
+      <c r="E5">
+        <v>62</v>
+      </c>
+      <c r="F5">
+        <v>51</v>
+      </c>
+      <c r="G5">
+        <v>44</v>
+      </c>
+      <c r="H5">
+        <v>38</v>
+      </c>
+      <c r="I5">
+        <v>34</v>
+      </c>
+      <c r="J5">
+        <v>31</v>
+      </c>
+      <c r="K5">
+        <v>29</v>
+      </c>
+      <c r="L5">
+        <v>26</v>
+      </c>
+      <c r="M5">
+        <v>24</v>
+      </c>
+      <c r="N5">
+        <v>22</v>
+      </c>
+      <c r="O5">
+        <v>21</v>
+      </c>
+      <c r="P5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>6248</v>
+      </c>
+      <c r="C7">
+        <v>6298</v>
+      </c>
+      <c r="D7">
+        <v>6324</v>
+      </c>
+      <c r="E7">
+        <v>6338</v>
+      </c>
+      <c r="F7">
+        <v>6349</v>
+      </c>
+      <c r="G7">
+        <v>6356</v>
+      </c>
+      <c r="H7">
+        <v>6362</v>
+      </c>
+      <c r="I7">
+        <v>6366</v>
+      </c>
+      <c r="J7">
+        <v>6369</v>
+      </c>
+      <c r="K7">
+        <v>6371</v>
+      </c>
+      <c r="L7">
+        <v>6374</v>
+      </c>
+      <c r="M7">
+        <v>6376</v>
+      </c>
+      <c r="N7">
+        <v>6378</v>
+      </c>
+      <c r="O7">
+        <v>6379</v>
+      </c>
+      <c r="P7">
+        <v>6381</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>56632</v>
+      </c>
+      <c r="C8">
+        <v>19342</v>
+      </c>
+      <c r="D8">
+        <v>54638</v>
+      </c>
+      <c r="E8">
+        <v>15238</v>
+      </c>
+      <c r="F8">
+        <v>9844</v>
+      </c>
+      <c r="G8">
+        <v>10049</v>
+      </c>
+      <c r="H8">
+        <v>57482</v>
+      </c>
+      <c r="I8">
+        <v>9130</v>
+      </c>
+      <c r="J8">
+        <v>9210</v>
+      </c>
+      <c r="K8">
+        <v>10603</v>
+      </c>
+      <c r="L8">
+        <v>9698</v>
+      </c>
+      <c r="M8">
+        <v>8915</v>
+      </c>
+      <c r="N8">
+        <v>11070</v>
+      </c>
+      <c r="O8">
+        <v>38105</v>
+      </c>
+      <c r="P8">
+        <v>64399</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>12176</v>
+      </c>
+      <c r="C9">
+        <v>5781</v>
+      </c>
+      <c r="D9">
+        <v>9878</v>
+      </c>
+      <c r="E9">
+        <v>4774</v>
+      </c>
+      <c r="F9">
+        <v>2639</v>
+      </c>
+      <c r="G9">
+        <v>2947</v>
+      </c>
+      <c r="H9">
+        <v>10179</v>
+      </c>
+      <c r="I9">
+        <v>2371</v>
+      </c>
+      <c r="J9">
+        <v>2547</v>
+      </c>
+      <c r="K9">
+        <v>3032</v>
+      </c>
+      <c r="L9">
+        <v>2547</v>
+      </c>
+      <c r="M9">
+        <v>2455</v>
+      </c>
+      <c r="N9">
+        <v>3421</v>
+      </c>
+      <c r="O9">
+        <v>9365</v>
+      </c>
+      <c r="P9">
+        <v>13159</v>
+      </c>
+    </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I10" t="s">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>94464</v>
+      </c>
+      <c r="C10">
+        <v>131754</v>
+      </c>
+      <c r="D10">
+        <v>96458</v>
+      </c>
+      <c r="E10">
+        <v>135858</v>
+      </c>
+      <c r="F10">
+        <v>141252</v>
+      </c>
+      <c r="G10">
+        <v>141047</v>
+      </c>
+      <c r="H10">
+        <v>93614</v>
+      </c>
+      <c r="I10">
+        <v>141966</v>
+      </c>
+      <c r="J10">
+        <v>141886</v>
+      </c>
+      <c r="K10">
+        <v>140493</v>
+      </c>
+      <c r="L10">
+        <v>141398</v>
+      </c>
+      <c r="M10">
+        <v>142181</v>
+      </c>
+      <c r="N10">
+        <v>140026</v>
+      </c>
+      <c r="O10">
+        <v>112991</v>
+      </c>
+      <c r="P10">
+        <v>86697</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
         <v>4</v>
       </c>
-      <c r="J10">
+      <c r="J16">
         <v>5200</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I11" t="s">
+    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
         <v>5</v>
       </c>
-      <c r="J11">
+      <c r="J17">
         <v>1200</v>
       </c>
     </row>

</xml_diff>